<commit_message>
Done clip c04 cart 07: Xay dung sươn class product repository
</commit_message>
<xml_diff>
--- a/MoTaDuAn.xlsx
+++ b/MoTaDuAn.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Class</t>
   </si>
@@ -53,13 +53,53 @@
   </si>
   <si>
     <t>boolean</t>
+  </si>
+  <si>
+    <t>ProductRepository</t>
+  </si>
+  <si>
+    <t>Proudct[]</t>
+  </si>
+  <si>
+    <t>Chứa danh sách các sản phẩm</t>
+  </si>
+  <si>
+    <t>Thêm mới sản phẩm</t>
+  </si>
+  <si>
+    <t>Add()</t>
+  </si>
+  <si>
+    <t>Phương thức</t>
+  </si>
+  <si>
+    <t>getItems</t>
+  </si>
+  <si>
+    <t>Lấy sản phẩm trong kho hàng</t>
+  </si>
+  <si>
+    <t>getItemByID</t>
+  </si>
+  <si>
+    <t>Lấy sản phẩm trong kho hàng
+dựa vào id</t>
+  </si>
+  <si>
+    <t>Mô tả</t>
+  </si>
+  <si>
+    <t>showItemsHTML()</t>
+  </si>
+  <si>
+    <t>Lấy sản phẩm hiển thị ra html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,7 +120,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -96,6 +136,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -127,13 +173,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -141,6 +183,32 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -157,6 +225,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Capture.JPG"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2200276"/>
+          <a:ext cx="6515100" cy="2962274"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -202,7 +313,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -234,10 +345,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -269,7 +379,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -445,85 +554,219 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7:G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="26.25">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-    </row>
-    <row r="2" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+    </row>
+    <row r="2" spans="1:16" ht="18.75">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:16" ht="18.75">
+      <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="5" t="s">
         <v>12</v>
       </c>
     </row>
+    <row r="5" spans="1:16" ht="26.25">
+      <c r="A5" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+    </row>
+    <row r="6" spans="1:16" ht="18.75">
+      <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+    </row>
+    <row r="7" spans="1:16" ht="18.75" customHeight="1">
+      <c r="A7" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="15"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="13">
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="N7:P8"/>
+    <mergeCell ref="B5:P5"/>
+    <mergeCell ref="H7:J8"/>
+    <mergeCell ref="E7:G8"/>
+    <mergeCell ref="B7:D8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="K7:M8"/>
     <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Done clip c04 cart 08: Xong phần sườn class card
</commit_message>
<xml_diff>
--- a/MoTaDuAn.xlsx
+++ b/MoTaDuAn.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Product" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
   <si>
     <t>Class</t>
   </si>
@@ -93,6 +93,21 @@
   </si>
   <si>
     <t>Lấy sản phẩm hiển thị ra html</t>
+  </si>
+  <si>
+    <t>CardItem</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Contructor (product: Productm quantity:number = 1)</t>
+  </si>
+  <si>
+    <t>ShowCarItemInHTML</t>
+  </si>
+  <si>
+    <t>getSubTotal()</t>
   </si>
 </sst>
 </file>
@@ -120,7 +135,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,8 +160,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -169,11 +190,74 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -184,31 +268,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -555,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P11"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:G8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32:G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -569,24 +687,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" ht="26.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
     </row>
     <row r="2" spans="1:16" ht="18.75">
       <c r="A2" s="2" t="s">
@@ -635,128 +753,213 @@
       </c>
     </row>
     <row r="5" spans="1:16" ht="26.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
     </row>
     <row r="6" spans="1:16" ht="18.75">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6" t="s">
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6" t="s">
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6" t="s">
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6" t="s">
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
     </row>
     <row r="7" spans="1:16" ht="18.75" customHeight="1">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
       <c r="H7" s="12" t="s">
         <v>20</v>
       </c>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
-      <c r="K7" s="13" t="s">
+      <c r="K7" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="8" t="s">
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="15"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
     </row>
     <row r="9" spans="1:16">
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:16">
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:16">
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="27" spans="1:7" ht="26.25">
+      <c r="A27" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+    </row>
+    <row r="28" spans="1:7" ht="18.75">
+      <c r="A28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="17"/>
+      <c r="D28" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="20"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+    </row>
+    <row r="29" spans="1:7" ht="18.75">
+      <c r="A29" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+    </row>
+    <row r="30" spans="1:7" ht="21" customHeight="1">
+      <c r="A30" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+    </row>
+    <row r="31" spans="1:7" ht="18.75" customHeight="1">
+      <c r="A31" s="26"/>
+      <c r="B31" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+    </row>
+    <row r="32" spans="1:7" ht="18.75" customHeight="1">
+      <c r="A32" s="27"/>
+      <c r="B32" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+    </row>
+    <row r="33" spans="2:7" ht="15" customHeight="1">
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="N7:P8"/>
-    <mergeCell ref="B5:P5"/>
-    <mergeCell ref="H7:J8"/>
-    <mergeCell ref="E7:G8"/>
-    <mergeCell ref="B7:D8"/>
+  <mergeCells count="22">
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B31:G31"/>
+    <mergeCell ref="B32:G32"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="K6:M6"/>
     <mergeCell ref="K7:M8"/>
@@ -764,6 +967,12 @@
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="H6:J6"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="N7:P8"/>
+    <mergeCell ref="B5:P5"/>
+    <mergeCell ref="H7:J8"/>
+    <mergeCell ref="E7:G8"/>
+    <mergeCell ref="B7:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Done clip c04 cart 09: Xây dung bo cuc cho class card
</commit_message>
<xml_diff>
--- a/MoTaDuAn.xlsx
+++ b/MoTaDuAn.xlsx
@@ -273,10 +273,53 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -284,49 +327,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -377,6 +377,44 @@
         <a:xfrm>
           <a:off x="0" y="2200276"/>
           <a:ext cx="6515100" cy="2962274"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>593912</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>33617</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="Capture.JPG"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="7351060"/>
+          <a:ext cx="6667500" cy="3653116"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -675,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32:G32"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M53" sqref="M53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -690,14 +728,14 @@
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
@@ -756,101 +794,101 @@
       <c r="A5" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
     </row>
     <row r="6" spans="1:16" ht="18.75">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9" t="s">
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9" t="s">
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9" t="s">
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9" t="s">
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
     </row>
     <row r="7" spans="1:16" ht="18.75" customHeight="1">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10" t="s">
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="12" t="s">
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="14" t="s">
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="10" t="s">
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="13"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
     </row>
     <row r="9" spans="1:16">
       <c r="B9" s="6"/>
@@ -871,86 +909,99 @@
       <c r="A27" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
     </row>
     <row r="28" spans="1:7" ht="18.75">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="19" t="s">
+      <c r="C28" s="15"/>
+      <c r="D28" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="20"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
     </row>
     <row r="29" spans="1:7" ht="18.75">
       <c r="A29" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
     </row>
     <row r="30" spans="1:7" ht="21" customHeight="1">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="24" t="s">
+      <c r="B30" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
     </row>
     <row r="31" spans="1:7" ht="18.75" customHeight="1">
-      <c r="A31" s="26"/>
-      <c r="B31" s="24" t="s">
+      <c r="A31" s="12"/>
+      <c r="B31" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
     </row>
     <row r="32" spans="1:7" ht="18.75" customHeight="1">
-      <c r="A32" s="27"/>
-      <c r="B32" s="24" t="s">
+      <c r="A32" s="13"/>
+      <c r="B32" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="24"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
     </row>
     <row r="33" spans="2:7" ht="15" customHeight="1">
-      <c r="B33" s="23"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="N7:P8"/>
+    <mergeCell ref="B5:P5"/>
+    <mergeCell ref="H7:J8"/>
+    <mergeCell ref="E7:G8"/>
+    <mergeCell ref="B7:D8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="K7:M8"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:J6"/>
     <mergeCell ref="A30:A32"/>
     <mergeCell ref="B27:G27"/>
     <mergeCell ref="B28:C28"/>
@@ -960,19 +1011,6 @@
     <mergeCell ref="B30:G30"/>
     <mergeCell ref="B31:G31"/>
     <mergeCell ref="B32:G32"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="K7:M8"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="N7:P8"/>
-    <mergeCell ref="B5:P5"/>
-    <mergeCell ref="H7:J8"/>
-    <mergeCell ref="E7:G8"/>
-    <mergeCell ref="B7:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Pendding c04 cart 16: 8:30
</commit_message>
<xml_diff>
--- a/MoTaDuAn.xlsx
+++ b/MoTaDuAn.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -113,8 +114,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,6 +278,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -286,9 +308,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -309,24 +328,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -469,7 +470,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -501,9 +502,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -535,6 +537,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -710,32 +713,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M53" sqref="M53"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" customWidth="1"/>
     <col min="6" max="6" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="26.25">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
@@ -744,7 +747,7 @@
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
     </row>
-    <row r="2" spans="1:16" ht="18.75">
+    <row r="2" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -767,7 +770,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="18.75">
+    <row r="3" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -790,196 +793,196 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="26.25">
+    <row r="5" spans="1:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A5" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-    </row>
-    <row r="6" spans="1:16" ht="18.75">
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+    </row>
+    <row r="6" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23" t="s">
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23" t="s">
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23" t="s">
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-    </row>
-    <row r="7" spans="1:16" ht="18.75" customHeight="1">
-      <c r="A7" s="22" t="s">
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+    </row>
+    <row r="7" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25" t="s">
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="27" t="s">
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="24" t="s">
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="25" t="s">
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="O7" s="25"/>
-      <c r="P7" s="25"/>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="22"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
-      <c r="P8" s="25"/>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
     </row>
-    <row r="27" spans="1:7" ht="26.25">
+    <row r="27" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A27" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-    </row>
-    <row r="28" spans="1:7" ht="18.75">
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+    </row>
+    <row r="28" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="17" t="s">
+      <c r="C28" s="21"/>
+      <c r="D28" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="18"/>
+      <c r="E28" s="24"/>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
     </row>
-    <row r="29" spans="1:7" ht="18.75">
+    <row r="29" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="20"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="26"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
     </row>
-    <row r="30" spans="1:7" ht="21" customHeight="1">
-      <c r="A30" s="11" t="s">
+    <row r="30" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="21" t="s">
+      <c r="B30" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-    </row>
-    <row r="31" spans="1:7" ht="18.75" customHeight="1">
-      <c r="A31" s="12"/>
-      <c r="B31" s="21" t="s">
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+    </row>
+    <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="19"/>
+      <c r="B31" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-    </row>
-    <row r="32" spans="1:7" ht="18.75" customHeight="1">
-      <c r="A32" s="13"/>
-      <c r="B32" s="21" t="s">
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+    </row>
+    <row r="32" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="20"/>
+      <c r="B32" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-    </row>
-    <row r="33" spans="2:7" ht="15" customHeight="1">
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+    </row>
+    <row r="33" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
@@ -989,19 +992,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="N7:P8"/>
-    <mergeCell ref="B5:P5"/>
-    <mergeCell ref="H7:J8"/>
-    <mergeCell ref="E7:G8"/>
-    <mergeCell ref="B7:D8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="K7:M8"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:J6"/>
     <mergeCell ref="A30:A32"/>
     <mergeCell ref="B27:G27"/>
     <mergeCell ref="B28:C28"/>
@@ -1011,9 +1001,34 @@
     <mergeCell ref="B30:G30"/>
     <mergeCell ref="B31:G31"/>
     <mergeCell ref="B32:G32"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="K7:M8"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="N7:P8"/>
+    <mergeCell ref="B5:P5"/>
+    <mergeCell ref="H7:J8"/>
+    <mergeCell ref="E7:G8"/>
+    <mergeCell ref="B7:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Done clip c04 cart 17: Khi click vào giá tiền hiển lấy ra id và số lượng của sản phẩm
</commit_message>
<xml_diff>
--- a/MoTaDuAn.xlsx
+++ b/MoTaDuAn.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="XayDungChucNangAddSanPham" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t>Class</t>
   </si>
@@ -109,13 +109,49 @@
   </si>
   <si>
     <t>getSubTotal()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bước 1: </t>
+  </si>
+  <si>
+    <t>Vừa vào trang</t>
+  </si>
+  <si>
+    <t>- Hiển thị danh sách sản phẩm</t>
+  </si>
+  <si>
+    <t>- Giỏ hàng rỗng</t>
+  </si>
+  <si>
+    <t>- Update thông báo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bước 2: </t>
+  </si>
+  <si>
+    <t>Khi click giá tiền</t>
+  </si>
+  <si>
+    <t>- Lấy id của sản phẩm</t>
+  </si>
+  <si>
+    <t>_ Truyền product.id vào data-product của thẻ a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_ Viết code lấy data-product </t>
+  </si>
+  <si>
+    <t>- Lấy quantity của sản phẩm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[&lt;=9999999][$-1000000]###\-####;[$-1000000]\(#\)\ ###\-####"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,8 +171,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="4"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -167,6 +209,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -258,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -278,10 +332,49 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -290,45 +383,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,6 +489,125 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>83710</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Capture.JPG"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="619126" y="1933576"/>
+          <a:ext cx="5991224" cy="1960134"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>609599</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>18238</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="Capture.JPG"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609599" y="4524375"/>
+          <a:ext cx="6018989" cy="1257300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>18271</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Capture.JPG"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="6429376"/>
+          <a:ext cx="6019021" cy="809624"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -470,7 +651,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -502,10 +683,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -537,7 +717,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -713,32 +892,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" customWidth="1"/>
     <col min="6" max="6" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="26.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
@@ -747,7 +926,7 @@
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
     </row>
-    <row r="2" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="18.75">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -770,7 +949,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="18.75">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -793,196 +972,196 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16" ht="26.25">
       <c r="A5" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-    </row>
-    <row r="6" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+    </row>
+    <row r="6" spans="1:16" ht="18.75">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11" t="s">
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11" t="s">
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11" t="s">
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11" t="s">
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-    </row>
-    <row r="7" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+    </row>
+    <row r="7" spans="1:16" ht="18.75" customHeight="1">
+      <c r="A7" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12" t="s">
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="14" t="s">
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="16" t="s">
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="12" t="s">
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="22"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="24"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+    </row>
+    <row r="9" spans="1:16">
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
     </row>
-    <row r="27" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:7" ht="26.25">
       <c r="A27" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-    </row>
-    <row r="28" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+    </row>
+    <row r="28" spans="1:7" ht="18.75">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="21"/>
-      <c r="D28" s="23" t="s">
+      <c r="C28" s="15"/>
+      <c r="D28" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="24"/>
+      <c r="E28" s="18"/>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
     </row>
-    <row r="29" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="18.75">
       <c r="A29" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="26"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="20"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
     </row>
-    <row r="30" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="18" t="s">
+    <row r="30" spans="1:7" ht="21" customHeight="1">
+      <c r="A30" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-    </row>
-    <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="19"/>
-      <c r="B31" s="27" t="s">
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+    </row>
+    <row r="31" spans="1:7" ht="18.75" customHeight="1">
+      <c r="A31" s="12"/>
+      <c r="B31" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-    </row>
-    <row r="32" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="20"/>
-      <c r="B32" s="27" t="s">
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+    </row>
+    <row r="32" spans="1:7" ht="18.75" customHeight="1">
+      <c r="A32" s="13"/>
+      <c r="B32" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="27"/>
-    </row>
-    <row r="33" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+    </row>
+    <row r="33" spans="2:7" ht="15" customHeight="1">
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
@@ -992,6 +1171,19 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="N7:P8"/>
+    <mergeCell ref="B5:P5"/>
+    <mergeCell ref="H7:J8"/>
+    <mergeCell ref="E7:G8"/>
+    <mergeCell ref="B7:D8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="K7:M8"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:J6"/>
     <mergeCell ref="A30:A32"/>
     <mergeCell ref="B27:G27"/>
     <mergeCell ref="B28:C28"/>
@@ -1001,19 +1193,6 @@
     <mergeCell ref="B30:G30"/>
     <mergeCell ref="B31:G31"/>
     <mergeCell ref="B32:G32"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="K7:M8"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="N7:P8"/>
-    <mergeCell ref="B5:P5"/>
-    <mergeCell ref="H7:J8"/>
-    <mergeCell ref="E7:G8"/>
-    <mergeCell ref="B7:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1022,13 +1201,214 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:E5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="18.75"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="28"/>
+    <col min="2" max="2" width="16.85546875" style="28" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="28"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="B2" s="29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="B3" s="29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="B4" s="29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="B6" s="29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="B7" s="29"/>
+      <c r="C7" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="29"/>
+      <c r="C18" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+    </row>
+    <row r="21" spans="2:6">
+      <c r="B21" s="33"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+    </row>
+    <row r="22" spans="2:6">
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+    </row>
+    <row r="23" spans="2:6">
+      <c r="B23" s="33"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+    </row>
+    <row r="24" spans="2:6">
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+    </row>
+    <row r="26" spans="2:6">
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+    </row>
+    <row r="27" spans="2:6">
+      <c r="B27" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B5:E5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Done clip c04 cart 18: validate cho phần input số lượng
</commit_message>
<xml_diff>
--- a/MoTaDuAn.xlsx
+++ b/MoTaDuAn.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
   <si>
     <t>Class</t>
   </si>
@@ -142,16 +142,28 @@
   </si>
   <si>
     <t>- Lấy quantity của sản phẩm</t>
+  </si>
+  <si>
+    <t>Class libs/validate.ts</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Validate cho input sản phẩm.</t>
+  </si>
+  <si>
+    <t>Hàm checkQuantity</t>
+  </si>
+  <si>
+    <t>Tiến hành kiểm tra sản phẩm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[&lt;=9999999][$-1000000]###\-####;[$-1000000]\(#\)\ ###\-####"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -332,65 +344,65 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,10 +511,10 @@
       <xdr:rowOff>28576</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>83710</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>232003</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -520,7 +532,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="619126" y="1933576"/>
-          <a:ext cx="5991224" cy="1960134"/>
+          <a:ext cx="7172324" cy="2346552"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -533,13 +545,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>18238</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -571,14 +583,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>18271</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -595,8 +607,140 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="609600" y="6429376"/>
+          <a:off x="609600" y="6677026"/>
           <a:ext cx="6019021" cy="809624"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>32607</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="8572500"/>
+          <a:ext cx="6000750" cy="1699482"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>168624</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609601" y="10953750"/>
+          <a:ext cx="6038850" cy="1597374"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>13925</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609601" y="13335001"/>
+          <a:ext cx="6014674" cy="1857374"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -651,7 +795,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -683,9 +827,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -717,6 +862,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -892,32 +1038,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" customWidth="1"/>
     <col min="6" max="6" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="26.25">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
@@ -926,7 +1072,7 @@
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
     </row>
-    <row r="2" spans="1:16" ht="18.75">
+    <row r="2" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -949,7 +1095,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="18.75">
+    <row r="3" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -972,196 +1118,196 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="26.25">
+    <row r="5" spans="1:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A5" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-    </row>
-    <row r="6" spans="1:16" ht="18.75">
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+    </row>
+    <row r="6" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23" t="s">
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23" t="s">
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23" t="s">
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23" t="s">
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-    </row>
-    <row r="7" spans="1:16" ht="18.75" customHeight="1">
-      <c r="A7" s="22" t="s">
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+    </row>
+    <row r="7" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25" t="s">
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="27" t="s">
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="24" t="s">
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="25" t="s">
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="O7" s="25"/>
-      <c r="P7" s="25"/>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="22"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
-      <c r="P8" s="25"/>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
     </row>
-    <row r="27" spans="1:7" ht="26.25">
+    <row r="27" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A27" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-    </row>
-    <row r="28" spans="1:7" ht="18.75">
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+    </row>
+    <row r="28" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="17" t="s">
+      <c r="C28" s="26"/>
+      <c r="D28" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="18"/>
+      <c r="E28" s="29"/>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
     </row>
-    <row r="29" spans="1:7" ht="18.75">
+    <row r="29" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="20"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="31"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
     </row>
-    <row r="30" spans="1:7" ht="21" customHeight="1">
-      <c r="A30" s="11" t="s">
+    <row r="30" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="21" t="s">
+      <c r="B30" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-    </row>
-    <row r="31" spans="1:7" ht="18.75" customHeight="1">
-      <c r="A31" s="12"/>
-      <c r="B31" s="21" t="s">
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+    </row>
+    <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="24"/>
+      <c r="B31" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-    </row>
-    <row r="32" spans="1:7" ht="18.75" customHeight="1">
-      <c r="A32" s="13"/>
-      <c r="B32" s="21" t="s">
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
+    </row>
+    <row r="32" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="25"/>
+      <c r="B32" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-    </row>
-    <row r="33" spans="2:7" ht="15" customHeight="1">
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+    </row>
+    <row r="33" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
@@ -1171,19 +1317,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="N7:P8"/>
-    <mergeCell ref="B5:P5"/>
-    <mergeCell ref="H7:J8"/>
-    <mergeCell ref="E7:G8"/>
-    <mergeCell ref="B7:D8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="K7:M8"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:J6"/>
     <mergeCell ref="A30:A32"/>
     <mergeCell ref="B27:G27"/>
     <mergeCell ref="B28:C28"/>
@@ -1193,6 +1326,19 @@
     <mergeCell ref="B30:G30"/>
     <mergeCell ref="B31:G31"/>
     <mergeCell ref="B32:G32"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="K7:M8"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="N7:P8"/>
+    <mergeCell ref="B5:P5"/>
+    <mergeCell ref="H7:J8"/>
+    <mergeCell ref="E7:G8"/>
+    <mergeCell ref="B7:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1201,206 +1347,240 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:E5"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="28"/>
-    <col min="2" max="2" width="16.85546875" style="28" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="28"/>
+    <col min="1" max="1" width="9.140625" style="11"/>
+    <col min="2" max="2" width="16.85546875" style="11" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="B2" s="29" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="B3" s="29" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="B4" s="29" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B4" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="31" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="B6" s="29" t="s">
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="12" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="B7" s="29"/>
-      <c r="C7" s="29" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="12"/>
+      <c r="C7" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-    </row>
-    <row r="17" spans="2:6">
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-    </row>
-    <row r="18" spans="2:6">
-      <c r="B18" s="29"/>
-      <c r="C18" s="29" t="s">
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B20" s="12"/>
+      <c r="C20" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-    </row>
-    <row r="19" spans="2:6">
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-    </row>
-    <row r="20" spans="2:6">
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-    </row>
-    <row r="21" spans="2:6">
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-    </row>
-    <row r="22" spans="2:6">
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-    </row>
-    <row r="23" spans="2:6">
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-    </row>
-    <row r="24" spans="2:6">
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-    </row>
-    <row r="25" spans="2:6">
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-    </row>
-    <row r="26" spans="2:6">
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-    </row>
-    <row r="27" spans="2:6">
-      <c r="B27" s="29" t="s">
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B29" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B37" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B47" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B57" s="11" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Done clip c04 cart 19: Đang phần thêm sản phẩm vào giỏ hàng phương thức addProduct
</commit_message>
<xml_diff>
--- a/MoTaDuAn.xlsx
+++ b/MoTaDuAn.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
   <si>
     <t>Class</t>
   </si>
@@ -129,9 +129,6 @@
     <t xml:space="preserve">Bước 2: </t>
   </si>
   <si>
-    <t>Khi click giá tiền</t>
-  </si>
-  <si>
     <t>- Lấy id của sản phẩm</t>
   </si>
   <si>
@@ -144,9 +141,6 @@
     <t>- Lấy quantity của sản phẩm</t>
   </si>
   <si>
-    <t>Class libs/validate.ts</t>
-  </si>
-  <si>
     <t xml:space="preserve"> - Validate cho input sản phẩm.</t>
   </si>
   <si>
@@ -154,16 +148,31 @@
   </si>
   <si>
     <t>Tiến hành kiểm tra sản phẩm</t>
+  </si>
+  <si>
+    <t>B1: Khi click giá tiền</t>
+  </si>
+  <si>
+    <t>B2: Thêm sản phẩm vào giỏ hàng</t>
+  </si>
+  <si>
+    <t>_ Mỗi sản phẩm thêm vào giỏ hàng tương đương 1 đối tượng CartItem</t>
+  </si>
+  <si>
+    <t>_ Cart có nhiều CartItem</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =&gt; Class libs/validate.ts</t>
+  </si>
+  <si>
+    <t>= &gt; Class libs/validate.ts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[&lt;=9999999][$-1000000]###\-####;[$-1000000]\(#\)\ ###\-####"/>
-  </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -344,15 +353,50 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -361,48 +405,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -641,7 +648,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -663,16 +670,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>600076</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>38101</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>168624</xdr:rowOff>
+      <xdr:colOff>28576</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>82899</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -685,7 +692,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -695,7 +702,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="609601" y="10953750"/>
+          <a:off x="600076" y="11582400"/>
           <a:ext cx="6038850" cy="1597374"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -729,7 +736,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -795,7 +802,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -827,10 +834,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -862,7 +868,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1038,32 +1043,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" customWidth="1"/>
     <col min="6" max="6" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="26.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
@@ -1072,7 +1077,7 @@
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
     </row>
-    <row r="2" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="18.75">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1095,7 +1100,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="18.75">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -1118,196 +1123,196 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16" ht="26.25">
       <c r="A5" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="18"/>
-    </row>
-    <row r="6" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="27"/>
+    </row>
+    <row r="6" spans="1:16" ht="18.75">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16" t="s">
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16" t="s">
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16" t="s">
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16" t="s">
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="O6" s="16"/>
-      <c r="P6" s="16"/>
-    </row>
-    <row r="7" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="O6" s="24"/>
+      <c r="P6" s="24"/>
+    </row>
+    <row r="7" spans="1:16" ht="18.75" customHeight="1">
+      <c r="A7" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17" t="s">
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="19" t="s">
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="21" t="s">
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="17" t="s">
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O7" s="26"/>
+      <c r="P7" s="26"/>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="23"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="26"/>
+    </row>
+    <row r="9" spans="1:16">
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
     </row>
-    <row r="27" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:7" ht="26.25">
       <c r="A27" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-    </row>
-    <row r="28" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+    </row>
+    <row r="28" spans="1:7" ht="18.75">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="26"/>
-      <c r="D28" s="28" t="s">
+      <c r="C28" s="16"/>
+      <c r="D28" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="29"/>
+      <c r="E28" s="19"/>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
     </row>
-    <row r="29" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="18.75">
       <c r="A29" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="31"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="21"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
     </row>
-    <row r="30" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="23" t="s">
+    <row r="30" spans="1:7" ht="21" customHeight="1">
+      <c r="A30" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="32" t="s">
+      <c r="B30" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="32"/>
-    </row>
-    <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="24"/>
-      <c r="B31" s="32" t="s">
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+    </row>
+    <row r="31" spans="1:7" ht="18.75" customHeight="1">
+      <c r="A31" s="13"/>
+      <c r="B31" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
-    </row>
-    <row r="32" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="25"/>
-      <c r="B32" s="32" t="s">
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+    </row>
+    <row r="32" spans="1:7" ht="18.75" customHeight="1">
+      <c r="A32" s="14"/>
+      <c r="B32" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="32"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="32"/>
-    </row>
-    <row r="33" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+    </row>
+    <row r="33" spans="2:7" ht="15" customHeight="1">
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
@@ -1317,6 +1322,19 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="N7:P8"/>
+    <mergeCell ref="B5:P5"/>
+    <mergeCell ref="H7:J8"/>
+    <mergeCell ref="E7:G8"/>
+    <mergeCell ref="B7:D8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="K7:M8"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:J6"/>
     <mergeCell ref="A30:A32"/>
     <mergeCell ref="B27:G27"/>
     <mergeCell ref="B28:C28"/>
@@ -1326,19 +1344,6 @@
     <mergeCell ref="B30:G30"/>
     <mergeCell ref="B31:G31"/>
     <mergeCell ref="B32:G32"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="K7:M8"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="N7:P8"/>
-    <mergeCell ref="B5:P5"/>
-    <mergeCell ref="H7:J8"/>
-    <mergeCell ref="E7:G8"/>
-    <mergeCell ref="B7:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1347,245 +1352,125 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G57"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="11"/>
     <col min="2" max="2" width="16.85546875" style="11" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="B2" s="11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="12" t="s">
+    <row r="3" spans="1:5">
+      <c r="B3" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="12" t="s">
+    <row r="4" spans="1:5">
+      <c r="B4" s="11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:5">
+      <c r="A5" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="B6" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="12" t="s">
+    </row>
+    <row r="7" spans="1:5">
+      <c r="C7" s="11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="12"/>
-      <c r="C7" s="12" t="s">
+    <row r="20" spans="2:3">
+      <c r="C20" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="12"/>
-      <c r="C20" s="12" t="s">
+    </row>
+    <row r="29" spans="2:3">
+      <c r="B29" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B29" s="12" t="s">
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B36" s="11" t="s">
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2">
+      <c r="B47" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2">
+      <c r="B48" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2">
+      <c r="B57" s="11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B37" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B47" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B57" s="11" t="s">
+    <row r="68" spans="2:5">
+      <c r="B68" s="30" t="s">
         <v>45</v>
       </c>
+      <c r="C68" s="30"/>
+      <c r="D68" s="30"/>
+      <c r="E68" s="30"/>
+    </row>
+    <row r="69" spans="2:5">
+      <c r="B69" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5">
+      <c r="B71" s="11" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B68:E68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Done c04 cart 21: Xay dung giao dien và kiem tra empty
</commit_message>
<xml_diff>
--- a/MoTaDuAn.xlsx
+++ b/MoTaDuAn.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
   <si>
     <t>Class</t>
   </si>
@@ -166,13 +166,28 @@
   </si>
   <si>
     <t>= &gt; Class libs/validate.ts</t>
+  </si>
+  <si>
+    <t>16/01/2018</t>
+  </si>
+  <si>
+    <t>: Viết thương thức thêm sản phẩm vào giỏ hảng</t>
+  </si>
+  <si>
+    <t>B1: Tiến hành kiểm tra</t>
+  </si>
+  <si>
+    <t>cart.ts</t>
+  </si>
+  <si>
+    <t>B2: Phương thức thêm vào giỏ hàng</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,6 +210,12 @@
     <font>
       <sz val="14"/>
       <color theme="4"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="9" tint="-0.499984740745262"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -333,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -354,6 +375,29 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -363,9 +407,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -387,29 +428,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -648,7 +670,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -692,7 +714,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -736,7 +758,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -748,6 +770,94 @@
         <a:xfrm>
           <a:off x="609601" y="13335001"/>
           <a:ext cx="6014674" cy="1857374"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>4266</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="17859376"/>
+          <a:ext cx="6005016" cy="2286000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>607533</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609601" y="20955001"/>
+          <a:ext cx="5998682" cy="2828924"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -802,7 +912,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -834,9 +944,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -868,6 +979,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1043,32 +1155,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" customWidth="1"/>
     <col min="6" max="6" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="26.25">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
@@ -1077,7 +1189,7 @@
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
     </row>
-    <row r="2" spans="1:16" ht="18.75">
+    <row r="2" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1100,7 +1212,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="18.75">
+    <row r="3" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -1123,196 +1235,196 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="26.25">
+    <row r="5" spans="1:16" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A5" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="27"/>
-      <c r="P5" s="27"/>
-    </row>
-    <row r="6" spans="1:16" ht="18.75">
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+    </row>
+    <row r="6" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24" t="s">
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24" t="s">
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24" t="s">
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-    </row>
-    <row r="7" spans="1:16" ht="18.75" customHeight="1">
-      <c r="A7" s="23" t="s">
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+    </row>
+    <row r="7" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26" t="s">
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="28" t="s">
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="25" t="s">
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="26" t="s">
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="O7" s="26"/>
-      <c r="P7" s="26"/>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="23"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="26"/>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
     </row>
-    <row r="27" spans="1:7" ht="26.25">
+    <row r="27" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A27" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-    </row>
-    <row r="28" spans="1:7" ht="18.75">
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+    </row>
+    <row r="28" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="18" t="s">
+      <c r="C28" s="24"/>
+      <c r="D28" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="19"/>
+      <c r="E28" s="27"/>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
     </row>
-    <row r="29" spans="1:7" ht="18.75">
+    <row r="29" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="21"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="29"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
     </row>
-    <row r="30" spans="1:7" ht="21" customHeight="1">
-      <c r="A30" s="12" t="s">
+    <row r="30" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
-    </row>
-    <row r="31" spans="1:7" ht="18.75" customHeight="1">
-      <c r="A31" s="13"/>
-      <c r="B31" s="22" t="s">
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+    </row>
+    <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="22"/>
+      <c r="B31" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-    </row>
-    <row r="32" spans="1:7" ht="18.75" customHeight="1">
-      <c r="A32" s="14"/>
-      <c r="B32" s="22" t="s">
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="30"/>
+    </row>
+    <row r="32" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="23"/>
+      <c r="B32" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-    </row>
-    <row r="33" spans="2:7" ht="15" customHeight="1">
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="30"/>
+    </row>
+    <row r="33" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
@@ -1322,19 +1434,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="N7:P8"/>
-    <mergeCell ref="B5:P5"/>
-    <mergeCell ref="H7:J8"/>
-    <mergeCell ref="E7:G8"/>
-    <mergeCell ref="B7:D8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="K7:M8"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:J6"/>
     <mergeCell ref="A30:A32"/>
     <mergeCell ref="B27:G27"/>
     <mergeCell ref="B28:C28"/>
@@ -1344,6 +1443,19 @@
     <mergeCell ref="B30:G30"/>
     <mergeCell ref="B31:G31"/>
     <mergeCell ref="B32:G32"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="K7:M8"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="N7:P8"/>
+    <mergeCell ref="B5:P5"/>
+    <mergeCell ref="H7:J8"/>
+    <mergeCell ref="E7:G8"/>
+    <mergeCell ref="B7:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1352,118 +1464,146 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="11"/>
     <col min="2" max="2" width="16.85546875" style="11" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B3" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" s="11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="31" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C7" s="11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C20" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="2:3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="2:2">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="2:2">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="2:2">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B47" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="48" spans="2:2">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B48" s="11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="57" spans="2:2">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B57" s="11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="68" spans="2:5">
-      <c r="B68" s="30" t="s">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B68" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C68" s="30"/>
-      <c r="D68" s="30"/>
-      <c r="E68" s="30"/>
-    </row>
-    <row r="69" spans="2:5">
+      <c r="C68" s="31"/>
+      <c r="D68" s="31"/>
+      <c r="E68" s="31"/>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B69" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="71" spans="2:5">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B71" s="11" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B73" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C73" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B74" s="11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B75" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B87" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B88" s="11" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>